<commit_message>
test filter statement type
</commit_message>
<xml_diff>
--- a/tests/data/demonstracoes.xlsx
+++ b/tests/data/demonstracoes.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mtsraposo/dev/central_balancos_py/tests/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74669EEA-5F1F-404F-AA47-50EC990C22C7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5F9A17E-AD07-C84E-87B9-5E149B772D66}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="35840" windowHeight="21900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="22">
   <si>
     <t>cnpj</t>
   </si>
@@ -80,6 +80,12 @@
   </si>
   <si>
     <t>APPLE</t>
+  </si>
+  <si>
+    <t>Balanço Patrimonial (BP)</t>
+  </si>
+  <si>
+    <t>Demonstração do Resultado do Exercício (DRE)</t>
   </si>
 </sst>
 </file>
@@ -118,7 +124,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -136,6 +142,32 @@
       <top style="thin">
         <color auto="1"/>
       </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
       <bottom style="thin">
         <color auto="1"/>
       </bottom>
@@ -149,7 +181,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -158,7 +190,10 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
@@ -469,7 +504,7 @@
   <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -510,7 +545,7 @@
       <c r="A2" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="3" t="s">
         <v>8</v>
       </c>
       <c r="C2" s="1" t="s">
@@ -530,8 +565,10 @@
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A3" s="4"/>
-      <c r="B3" s="4"/>
+      <c r="A3" s="5"/>
+      <c r="B3" s="3" t="s">
+        <v>20</v>
+      </c>
       <c r="C3" s="1" t="s">
         <v>10</v>
       </c>
@@ -553,7 +590,7 @@
         <v>19</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>8</v>
+        <v>21</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>17</v>
@@ -572,9 +609,8 @@
       </c>
     </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="1">
     <mergeCell ref="A2:A3"/>
-    <mergeCell ref="B2:B3"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="G2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
@@ -582,5 +618,6 @@
     <hyperlink ref="G4" r:id="rId3" xr:uid="{1DA6EA90-D97E-0846-94BE-43A7EDBABAC5}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>